<commit_message>
Final commit with 4 testcases
</commit_message>
<xml_diff>
--- a/DemoTwitterProject/data/TC002.xlsx
+++ b/DemoTwitterProject/data/TC002.xlsx
@@ -25,13 +25,13 @@
     <t>emailID</t>
   </si>
   <si>
-    <t>TestingLE</t>
-  </si>
-  <si>
-    <t>testersample@xyz.com</t>
-  </si>
-  <si>
     <t>Aldod@334;</t>
+  </si>
+  <si>
+    <t>TesdgsLE</t>
+  </si>
+  <si>
+    <t>testersvbsksle@xyz.com</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,13 +417,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>